<commit_message>
Enhance SQL scripts by adding new EMA cross conditions, renaming columns for clarity, and updating queries for improved data retrieval
</commit_message>
<xml_diff>
--- a/Database_Scripts/Analysis of Stocks/Calculation of Fields-v1.xlsx
+++ b/Database_Scripts/Analysis of Stocks/Calculation of Fields-v1.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsrsr\Documents\SQL Server Management Studio\Analysis of Stocks\Analysis of Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsrsr\Documents\PythonProject\Database_Scripts\Analysis of Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD1CBCC-4068-4320-A5B9-2603FCA866C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DF0701-E55A-4892-B04B-58880E147745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AF0132B0-59B1-40C0-A0D0-BAF2B59667B3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{AF0132B0-59B1-40C0-A0D0-BAF2B59667B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Calculations" sheetId="1" r:id="rId1"/>
+    <sheet name="Sort order of Fields" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sort order of Fields'!$A$1:$G$191</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="426">
   <si>
     <t>Sno</t>
   </si>
@@ -1158,6 +1162,162 @@
   </si>
   <si>
     <t>new name</t>
+  </si>
+  <si>
+    <t>volume_15_minutes_shockers</t>
+  </si>
+  <si>
+    <t>volume_1_hourly_shockers</t>
+  </si>
+  <si>
+    <t>volume_4_hourly_shockers</t>
+  </si>
+  <si>
+    <t>volume_daily_shockers</t>
+  </si>
+  <si>
+    <t>volume_weekly_shockers</t>
+  </si>
+  <si>
+    <t>volume_monthly_shockers</t>
+  </si>
+  <si>
+    <t>volume_quarterly_shockers</t>
+  </si>
+  <si>
+    <t>volume_yearly_shockers</t>
+  </si>
+  <si>
+    <t>Ema_50_200_15_Minutes_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_15_Minutes_Crosses_Above</t>
+  </si>
+  <si>
+    <t>Ema_50_200_1_Hourly_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_1_Hourly_Crosses_Above</t>
+  </si>
+  <si>
+    <t>Ema_50_200_4_Hourly_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_4_Hourly_Crosses_Above</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Daily_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Daily_Crosses_Above</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Weekly_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Weekly_Crosses_Above</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Monthly_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Monthly_Crosses_Above</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Quarterly_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Quarterly_Crosses_Above</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Yearly_Crosses_Below</t>
+  </si>
+  <si>
+    <t>Ema_50_200_Yearly_Crosses_Above</t>
+  </si>
+  <si>
+    <t>INE263A01024</t>
+  </si>
+  <si>
+    <t>Percent_Change</t>
+  </si>
+  <si>
+    <t>Bharat Electronics Limited</t>
+  </si>
+  <si>
+    <t>Trade_Type_Details_Sum</t>
+  </si>
+  <si>
+    <t>Trade_Type_Details_Length</t>
+  </si>
+  <si>
+    <t>Bullish - Single Screen - Yearly;Bullish - Single Screen - Quarterly;Bullish - Double Screen - Strong - Quarterly;</t>
+  </si>
+  <si>
+    <t>Trade_Type_Details</t>
+  </si>
+  <si>
+    <t>Trade_Type_Bearish_Sum</t>
+  </si>
+  <si>
+    <t>Trade_Type_Bullish_Sum</t>
+  </si>
+  <si>
+    <t>Trade_Type_Length</t>
+  </si>
+  <si>
+    <t>Bullish;Bullish;Bullish;</t>
+  </si>
+  <si>
+    <t>Trade_Type</t>
+  </si>
+  <si>
+    <t>Trading_View_Order</t>
+  </si>
+  <si>
+    <t>Trading_View</t>
+  </si>
+  <si>
+    <t>Volume_Shockers_Sum</t>
+  </si>
+  <si>
+    <t>15minutes</t>
+  </si>
+  <si>
+    <t>Segments_Sum</t>
+  </si>
+  <si>
+    <t>Segments_Length</t>
+  </si>
+  <si>
+    <t>Segments_Order</t>
+  </si>
+  <si>
+    <t>Nifty 50;Nifty 100;Nifty 200;Nifty 500;Nifty 500 Large Mid Small Equal Cap Weighted;Nifty 500 Multi Cap 50:25:25;Nifty 500 Multi Cap India Manufacturing 50:30:20;Nifty Total Market;Nifty Large Mid Cap 250;Nifty CPSE;Nifty PSE;Nifty India Manufacturing;Nifty India Railways PSU;Futures;Cash</t>
+  </si>
+  <si>
+    <t>Capital Goods</t>
+  </si>
+  <si>
+    <t>BEL</t>
+  </si>
+  <si>
+    <t>03-08-2025  7:06:28 AM</t>
+  </si>
+  <si>
+    <t>Report_Sort_Order</t>
+  </si>
+  <si>
+    <t>20250803070622</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>column names</t>
+  </si>
+  <si>
+    <t>sno</t>
   </si>
 </sst>
 </file>
@@ -1212,12 +1372,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1554,7 +1717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D301AB36-4F54-4FD0-8F46-F2B6C47075AA}">
   <dimension ref="A2:M336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" workbookViewId="0">
+    <sheetView topLeftCell="C12" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -5785,7 +5948,7 @@
         <v>365</v>
       </c>
       <c r="E330" t="str">
-        <f t="shared" ref="E330:E393" si="5">VLOOKUP(J330,D:D,1,FALSE)</f>
+        <f t="shared" ref="E330:E334" si="5">VLOOKUP(J330,D:D,1,FALSE)</f>
         <v>volume__quarterly__shockers</v>
       </c>
       <c r="J330" t="s">
@@ -5868,4 +6031,3514 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6608BF70-2CA7-42CE-93FA-D05E242771BF}">
+  <dimension ref="A1:G191"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="5.109375" customWidth="1"/>
+    <col min="5" max="5" width="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>425</v>
+      </c>
+      <c r="B1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>17457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>421</v>
+      </c>
+      <c r="C4">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C9">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C10">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C11">
+        <v>7150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>370</v>
+      </c>
+      <c r="C12" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>412</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>411</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>410</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>409</v>
+      </c>
+      <c r="C16" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>407</v>
+      </c>
+      <c r="C17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>406</v>
+      </c>
+      <c r="C18">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>405</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>404</v>
+      </c>
+      <c r="C20" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>402</v>
+      </c>
+      <c r="C21">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>401</v>
+      </c>
+      <c r="C22">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>377.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>399</v>
+      </c>
+      <c r="C25">
+        <v>-1.54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26">
+        <v>8702605</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30">
+        <v>213</v>
+      </c>
+      <c r="F30" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31">
+        <v>214</v>
+      </c>
+      <c r="F31" t="s">
+        <v>104</v>
+      </c>
+      <c r="G31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32">
+        <v>215</v>
+      </c>
+      <c r="F32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33">
+        <v>216</v>
+      </c>
+      <c r="F33" t="s">
+        <v>106</v>
+      </c>
+      <c r="G33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34">
+        <v>217</v>
+      </c>
+      <c r="F34" t="s">
+        <v>107</v>
+      </c>
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35">
+        <v>218</v>
+      </c>
+      <c r="F35" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36">
+        <v>220</v>
+      </c>
+      <c r="F36" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>38</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37">
+        <v>221</v>
+      </c>
+      <c r="F37" t="s">
+        <v>110</v>
+      </c>
+      <c r="G37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>39</v>
+      </c>
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38">
+        <v>222</v>
+      </c>
+      <c r="F38" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39">
+        <v>223</v>
+      </c>
+      <c r="F39" t="s">
+        <v>112</v>
+      </c>
+      <c r="G39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40">
+        <v>224</v>
+      </c>
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>42</v>
+      </c>
+      <c r="B41" t="s">
+        <v>80</v>
+      </c>
+      <c r="C41" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41">
+        <v>225</v>
+      </c>
+      <c r="F41" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>227</v>
+      </c>
+      <c r="F42" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43">
+        <v>228</v>
+      </c>
+      <c r="F43" t="s">
+        <v>116</v>
+      </c>
+      <c r="G43" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44">
+        <v>229</v>
+      </c>
+      <c r="F44" t="s">
+        <v>117</v>
+      </c>
+      <c r="G44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C45" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45">
+        <v>230</v>
+      </c>
+      <c r="F45" t="s">
+        <v>118</v>
+      </c>
+      <c r="G45" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46">
+        <v>231</v>
+      </c>
+      <c r="F46" t="s">
+        <v>119</v>
+      </c>
+      <c r="G46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47">
+        <v>232</v>
+      </c>
+      <c r="F47" t="s">
+        <v>120</v>
+      </c>
+      <c r="G47" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48">
+        <v>233</v>
+      </c>
+      <c r="F48" t="s">
+        <v>121</v>
+      </c>
+      <c r="G48" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+      <c r="C49" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49">
+        <v>235</v>
+      </c>
+      <c r="F49" t="s">
+        <v>122</v>
+      </c>
+      <c r="G49" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>53</v>
+      </c>
+      <c r="B50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
+        <v>32</v>
+      </c>
+      <c r="E50">
+        <v>236</v>
+      </c>
+      <c r="F50" t="s">
+        <v>123</v>
+      </c>
+      <c r="G50" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>54</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+      <c r="C51" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51">
+        <v>237</v>
+      </c>
+      <c r="F51" t="s">
+        <v>124</v>
+      </c>
+      <c r="G51" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52">
+        <v>238</v>
+      </c>
+      <c r="F52" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>56</v>
+      </c>
+      <c r="B53" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" t="s">
+        <v>32</v>
+      </c>
+      <c r="E53">
+        <v>239</v>
+      </c>
+      <c r="F53" t="s">
+        <v>126</v>
+      </c>
+      <c r="G53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>57</v>
+      </c>
+      <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
+        <v>32</v>
+      </c>
+      <c r="E54">
+        <v>240</v>
+      </c>
+      <c r="F54" t="s">
+        <v>127</v>
+      </c>
+      <c r="G54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>58</v>
+      </c>
+      <c r="B55" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" t="s">
+        <v>32</v>
+      </c>
+      <c r="E55">
+        <v>241</v>
+      </c>
+      <c r="F55" t="s">
+        <v>128</v>
+      </c>
+      <c r="G55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>60</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="5">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>243</v>
+      </c>
+      <c r="F56" t="s">
+        <v>129</v>
+      </c>
+      <c r="G56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>61</v>
+      </c>
+      <c r="B57" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>244</v>
+      </c>
+      <c r="F57" t="s">
+        <v>130</v>
+      </c>
+      <c r="G57" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>62</v>
+      </c>
+      <c r="B58" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" t="s">
+        <v>32</v>
+      </c>
+      <c r="E58">
+        <v>245</v>
+      </c>
+      <c r="F58" t="s">
+        <v>131</v>
+      </c>
+      <c r="G58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>63</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>32</v>
+      </c>
+      <c r="E59">
+        <v>246</v>
+      </c>
+      <c r="F59" t="s">
+        <v>132</v>
+      </c>
+      <c r="G59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>64</v>
+      </c>
+      <c r="B60" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" t="s">
+        <v>32</v>
+      </c>
+      <c r="E60">
+        <v>247</v>
+      </c>
+      <c r="F60" t="s">
+        <v>133</v>
+      </c>
+      <c r="G60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>65</v>
+      </c>
+      <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61">
+        <v>248</v>
+      </c>
+      <c r="F61" t="s">
+        <v>134</v>
+      </c>
+      <c r="G61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>66</v>
+      </c>
+      <c r="B62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" t="s">
+        <v>32</v>
+      </c>
+      <c r="E62">
+        <v>249</v>
+      </c>
+      <c r="F62" t="s">
+        <v>135</v>
+      </c>
+      <c r="G62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>67</v>
+      </c>
+      <c r="B63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" t="s">
+        <v>32</v>
+      </c>
+      <c r="E63">
+        <v>250</v>
+      </c>
+      <c r="F63" t="s">
+        <v>136</v>
+      </c>
+      <c r="G63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>69</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C64" s="5">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>252</v>
+      </c>
+      <c r="F64" t="s">
+        <v>138</v>
+      </c>
+      <c r="G64" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>70</v>
+      </c>
+      <c r="B65" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <v>253</v>
+      </c>
+      <c r="F65" t="s">
+        <v>140</v>
+      </c>
+      <c r="G65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>71</v>
+      </c>
+      <c r="B66" t="s">
+        <v>141</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="E66">
+        <v>254</v>
+      </c>
+      <c r="F66" t="s">
+        <v>142</v>
+      </c>
+      <c r="G66" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>72</v>
+      </c>
+      <c r="B67" t="s">
+        <v>143</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>255</v>
+      </c>
+      <c r="F67" t="s">
+        <v>144</v>
+      </c>
+      <c r="G67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>73</v>
+      </c>
+      <c r="B68" t="s">
+        <v>145</v>
+      </c>
+      <c r="C68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68">
+        <v>256</v>
+      </c>
+      <c r="F68" t="s">
+        <v>146</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>74</v>
+      </c>
+      <c r="B69" t="s">
+        <v>147</v>
+      </c>
+      <c r="C69" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69">
+        <v>257</v>
+      </c>
+      <c r="F69" t="s">
+        <v>148</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>75</v>
+      </c>
+      <c r="B70" t="s">
+        <v>149</v>
+      </c>
+      <c r="C70" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70">
+        <v>258</v>
+      </c>
+      <c r="F70" t="s">
+        <v>150</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>76</v>
+      </c>
+      <c r="B71" t="s">
+        <v>151</v>
+      </c>
+      <c r="C71" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71">
+        <v>259</v>
+      </c>
+      <c r="F71" t="s">
+        <v>152</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>78</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C72" s="5">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>261</v>
+      </c>
+      <c r="F72" t="s">
+        <v>250</v>
+      </c>
+      <c r="G72" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>79</v>
+      </c>
+      <c r="B73" t="s">
+        <v>251</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>262</v>
+      </c>
+      <c r="F73" t="s">
+        <v>252</v>
+      </c>
+      <c r="G73" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>80</v>
+      </c>
+      <c r="B74" t="s">
+        <v>253</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="E74">
+        <v>263</v>
+      </c>
+      <c r="F74" t="s">
+        <v>254</v>
+      </c>
+      <c r="G74" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>81</v>
+      </c>
+      <c r="B75" t="s">
+        <v>255</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>264</v>
+      </c>
+      <c r="F75" t="s">
+        <v>256</v>
+      </c>
+      <c r="G75" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>82</v>
+      </c>
+      <c r="B76" t="s">
+        <v>257</v>
+      </c>
+      <c r="C76" t="s">
+        <v>32</v>
+      </c>
+      <c r="E76">
+        <v>265</v>
+      </c>
+      <c r="F76" t="s">
+        <v>258</v>
+      </c>
+      <c r="G76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>83</v>
+      </c>
+      <c r="B77" t="s">
+        <v>259</v>
+      </c>
+      <c r="C77" t="s">
+        <v>32</v>
+      </c>
+      <c r="E77">
+        <v>266</v>
+      </c>
+      <c r="F77" t="s">
+        <v>260</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>84</v>
+      </c>
+      <c r="B78" t="s">
+        <v>261</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="E78">
+        <v>267</v>
+      </c>
+      <c r="F78" t="s">
+        <v>262</v>
+      </c>
+      <c r="G78" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>85</v>
+      </c>
+      <c r="B79" t="s">
+        <v>263</v>
+      </c>
+      <c r="C79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>268</v>
+      </c>
+      <c r="F79" t="s">
+        <v>264</v>
+      </c>
+      <c r="G79" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>87</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C80" s="5">
+        <v>1</v>
+      </c>
+      <c r="E80">
+        <v>270</v>
+      </c>
+      <c r="F80" t="s">
+        <v>154</v>
+      </c>
+      <c r="G80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>88</v>
+      </c>
+      <c r="B81" t="s">
+        <v>155</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="E81">
+        <v>271</v>
+      </c>
+      <c r="F81" t="s">
+        <v>156</v>
+      </c>
+      <c r="G81" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>89</v>
+      </c>
+      <c r="B82" t="s">
+        <v>157</v>
+      </c>
+      <c r="C82" t="s">
+        <v>32</v>
+      </c>
+      <c r="E82">
+        <v>272</v>
+      </c>
+      <c r="F82" t="s">
+        <v>158</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>90</v>
+      </c>
+      <c r="B83" t="s">
+        <v>159</v>
+      </c>
+      <c r="C83" t="s">
+        <v>32</v>
+      </c>
+      <c r="E83">
+        <v>273</v>
+      </c>
+      <c r="F83" t="s">
+        <v>160</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>91</v>
+      </c>
+      <c r="B84" t="s">
+        <v>161</v>
+      </c>
+      <c r="C84" t="s">
+        <v>32</v>
+      </c>
+      <c r="E84">
+        <v>274</v>
+      </c>
+      <c r="F84" t="s">
+        <v>162</v>
+      </c>
+      <c r="G84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>92</v>
+      </c>
+      <c r="B85" t="s">
+        <v>163</v>
+      </c>
+      <c r="C85" t="s">
+        <v>32</v>
+      </c>
+      <c r="E85">
+        <v>275</v>
+      </c>
+      <c r="F85" t="s">
+        <v>164</v>
+      </c>
+      <c r="G85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>93</v>
+      </c>
+      <c r="B86" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" t="s">
+        <v>32</v>
+      </c>
+      <c r="E86">
+        <v>276</v>
+      </c>
+      <c r="F86" t="s">
+        <v>166</v>
+      </c>
+      <c r="G86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>94</v>
+      </c>
+      <c r="B87" t="s">
+        <v>167</v>
+      </c>
+      <c r="C87" t="s">
+        <v>32</v>
+      </c>
+      <c r="E87">
+        <v>277</v>
+      </c>
+      <c r="F87" t="s">
+        <v>168</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>96</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C88" s="5">
+        <v>1</v>
+      </c>
+      <c r="E88">
+        <v>279</v>
+      </c>
+      <c r="F88" t="s">
+        <v>170</v>
+      </c>
+      <c r="G88" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>97</v>
+      </c>
+      <c r="B89" t="s">
+        <v>171</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>280</v>
+      </c>
+      <c r="F89" t="s">
+        <v>172</v>
+      </c>
+      <c r="G89" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>98</v>
+      </c>
+      <c r="B90" t="s">
+        <v>173</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="E90">
+        <v>281</v>
+      </c>
+      <c r="F90" t="s">
+        <v>174</v>
+      </c>
+      <c r="G90" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>99</v>
+      </c>
+      <c r="B91" t="s">
+        <v>175</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>282</v>
+      </c>
+      <c r="F91" t="s">
+        <v>176</v>
+      </c>
+      <c r="G91" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>100</v>
+      </c>
+      <c r="B92" t="s">
+        <v>177</v>
+      </c>
+      <c r="C92" t="s">
+        <v>32</v>
+      </c>
+      <c r="E92">
+        <v>283</v>
+      </c>
+      <c r="F92" t="s">
+        <v>178</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>101</v>
+      </c>
+      <c r="B93" t="s">
+        <v>179</v>
+      </c>
+      <c r="C93" t="s">
+        <v>32</v>
+      </c>
+      <c r="E93">
+        <v>284</v>
+      </c>
+      <c r="F93" t="s">
+        <v>180</v>
+      </c>
+      <c r="G93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>102</v>
+      </c>
+      <c r="B94" t="s">
+        <v>181</v>
+      </c>
+      <c r="C94" t="s">
+        <v>32</v>
+      </c>
+      <c r="E94">
+        <v>285</v>
+      </c>
+      <c r="F94" t="s">
+        <v>182</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>103</v>
+      </c>
+      <c r="B95" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" t="s">
+        <v>32</v>
+      </c>
+      <c r="E95">
+        <v>286</v>
+      </c>
+      <c r="F95" t="s">
+        <v>184</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>105</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C96" s="5">
+        <v>1</v>
+      </c>
+      <c r="E96">
+        <v>288</v>
+      </c>
+      <c r="F96" t="s">
+        <v>186</v>
+      </c>
+      <c r="G96" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>106</v>
+      </c>
+      <c r="B97" t="s">
+        <v>187</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="E97">
+        <v>289</v>
+      </c>
+      <c r="F97" t="s">
+        <v>188</v>
+      </c>
+      <c r="G97" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>107</v>
+      </c>
+      <c r="B98" t="s">
+        <v>189</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="E98">
+        <v>290</v>
+      </c>
+      <c r="F98" t="s">
+        <v>190</v>
+      </c>
+      <c r="G98" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>108</v>
+      </c>
+      <c r="B99" t="s">
+        <v>191</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>291</v>
+      </c>
+      <c r="F99" t="s">
+        <v>192</v>
+      </c>
+      <c r="G99" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>109</v>
+      </c>
+      <c r="B100" t="s">
+        <v>193</v>
+      </c>
+      <c r="C100" t="s">
+        <v>32</v>
+      </c>
+      <c r="E100">
+        <v>292</v>
+      </c>
+      <c r="F100" t="s">
+        <v>194</v>
+      </c>
+      <c r="G100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>110</v>
+      </c>
+      <c r="B101" t="s">
+        <v>195</v>
+      </c>
+      <c r="C101" t="s">
+        <v>32</v>
+      </c>
+      <c r="E101">
+        <v>293</v>
+      </c>
+      <c r="F101" t="s">
+        <v>196</v>
+      </c>
+      <c r="G101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>111</v>
+      </c>
+      <c r="B102" t="s">
+        <v>197</v>
+      </c>
+      <c r="C102" t="s">
+        <v>32</v>
+      </c>
+      <c r="E102">
+        <v>294</v>
+      </c>
+      <c r="F102" t="s">
+        <v>198</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>112</v>
+      </c>
+      <c r="B103" t="s">
+        <v>199</v>
+      </c>
+      <c r="C103" t="s">
+        <v>32</v>
+      </c>
+      <c r="E103">
+        <v>295</v>
+      </c>
+      <c r="F103" t="s">
+        <v>200</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>114</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C104" s="5">
+        <v>1</v>
+      </c>
+      <c r="E104">
+        <v>297</v>
+      </c>
+      <c r="F104" t="s">
+        <v>202</v>
+      </c>
+      <c r="G104" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>115</v>
+      </c>
+      <c r="B105" t="s">
+        <v>203</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="E105">
+        <v>298</v>
+      </c>
+      <c r="F105" t="s">
+        <v>204</v>
+      </c>
+      <c r="G105" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>116</v>
+      </c>
+      <c r="B106" t="s">
+        <v>205</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="E106">
+        <v>299</v>
+      </c>
+      <c r="F106" t="s">
+        <v>206</v>
+      </c>
+      <c r="G106" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>117</v>
+      </c>
+      <c r="B107" t="s">
+        <v>207</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>300</v>
+      </c>
+      <c r="F107" t="s">
+        <v>208</v>
+      </c>
+      <c r="G107" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>118</v>
+      </c>
+      <c r="B108" t="s">
+        <v>209</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="E108">
+        <v>301</v>
+      </c>
+      <c r="F108" t="s">
+        <v>210</v>
+      </c>
+      <c r="G108" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>119</v>
+      </c>
+      <c r="B109" t="s">
+        <v>211</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>302</v>
+      </c>
+      <c r="F109" t="s">
+        <v>212</v>
+      </c>
+      <c r="G109" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>120</v>
+      </c>
+      <c r="B110" t="s">
+        <v>213</v>
+      </c>
+      <c r="C110" t="s">
+        <v>32</v>
+      </c>
+      <c r="E110">
+        <v>303</v>
+      </c>
+      <c r="F110" t="s">
+        <v>214</v>
+      </c>
+      <c r="G110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>121</v>
+      </c>
+      <c r="B111" t="s">
+        <v>215</v>
+      </c>
+      <c r="C111" t="s">
+        <v>32</v>
+      </c>
+      <c r="E111">
+        <v>304</v>
+      </c>
+      <c r="F111" t="s">
+        <v>216</v>
+      </c>
+      <c r="G111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>123</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C112" s="5">
+        <v>1</v>
+      </c>
+      <c r="E112">
+        <v>306</v>
+      </c>
+      <c r="F112" t="s">
+        <v>396</v>
+      </c>
+      <c r="G112" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>124</v>
+      </c>
+      <c r="B113" t="s">
+        <v>395</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="E113">
+        <v>307</v>
+      </c>
+      <c r="F113" t="s">
+        <v>394</v>
+      </c>
+      <c r="G113" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>125</v>
+      </c>
+      <c r="B114" t="s">
+        <v>393</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="E114">
+        <v>308</v>
+      </c>
+      <c r="F114" t="s">
+        <v>392</v>
+      </c>
+      <c r="G114" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>126</v>
+      </c>
+      <c r="B115" t="s">
+        <v>391</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="E115">
+        <v>309</v>
+      </c>
+      <c r="F115" t="s">
+        <v>390</v>
+      </c>
+      <c r="G115" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>127</v>
+      </c>
+      <c r="B116" t="s">
+        <v>389</v>
+      </c>
+      <c r="C116">
+        <v>1</v>
+      </c>
+      <c r="E116">
+        <v>310</v>
+      </c>
+      <c r="F116" t="s">
+        <v>388</v>
+      </c>
+      <c r="G116" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>128</v>
+      </c>
+      <c r="B117" t="s">
+        <v>387</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="E117">
+        <v>311</v>
+      </c>
+      <c r="F117" t="s">
+        <v>386</v>
+      </c>
+      <c r="G117" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>129</v>
+      </c>
+      <c r="B118" t="s">
+        <v>385</v>
+      </c>
+      <c r="C118" t="s">
+        <v>32</v>
+      </c>
+      <c r="E118">
+        <v>312</v>
+      </c>
+      <c r="F118" t="s">
+        <v>384</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>130</v>
+      </c>
+      <c r="B119" t="s">
+        <v>383</v>
+      </c>
+      <c r="C119" t="s">
+        <v>32</v>
+      </c>
+      <c r="E119">
+        <v>313</v>
+      </c>
+      <c r="F119" t="s">
+        <v>382</v>
+      </c>
+      <c r="G119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>132</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C120" s="5">
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>315</v>
+      </c>
+      <c r="F120" t="s">
+        <v>218</v>
+      </c>
+      <c r="G120" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>133</v>
+      </c>
+      <c r="B121" t="s">
+        <v>219</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>316</v>
+      </c>
+      <c r="F121" t="s">
+        <v>220</v>
+      </c>
+      <c r="G121" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>134</v>
+      </c>
+      <c r="B122" t="s">
+        <v>221</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>317</v>
+      </c>
+      <c r="F122" t="s">
+        <v>222</v>
+      </c>
+      <c r="G122" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>135</v>
+      </c>
+      <c r="B123" t="s">
+        <v>223</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>318</v>
+      </c>
+      <c r="F123" t="s">
+        <v>224</v>
+      </c>
+      <c r="G123" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>136</v>
+      </c>
+      <c r="B124" t="s">
+        <v>225</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>319</v>
+      </c>
+      <c r="F124" t="s">
+        <v>226</v>
+      </c>
+      <c r="G124" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>137</v>
+      </c>
+      <c r="B125" t="s">
+        <v>227</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="E125">
+        <v>320</v>
+      </c>
+      <c r="F125" t="s">
+        <v>228</v>
+      </c>
+      <c r="G125" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>138</v>
+      </c>
+      <c r="B126" t="s">
+        <v>229</v>
+      </c>
+      <c r="C126" t="s">
+        <v>32</v>
+      </c>
+      <c r="E126">
+        <v>321</v>
+      </c>
+      <c r="F126" t="s">
+        <v>230</v>
+      </c>
+      <c r="G126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>139</v>
+      </c>
+      <c r="B127" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" t="s">
+        <v>32</v>
+      </c>
+      <c r="E127">
+        <v>322</v>
+      </c>
+      <c r="F127" t="s">
+        <v>232</v>
+      </c>
+      <c r="G127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>141</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C128" s="5">
+        <v>1</v>
+      </c>
+      <c r="E128">
+        <v>324</v>
+      </c>
+      <c r="F128" t="s">
+        <v>234</v>
+      </c>
+      <c r="G128" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>142</v>
+      </c>
+      <c r="B129" t="s">
+        <v>235</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <v>325</v>
+      </c>
+      <c r="F129" t="s">
+        <v>236</v>
+      </c>
+      <c r="G129" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>143</v>
+      </c>
+      <c r="B130" t="s">
+        <v>237</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>326</v>
+      </c>
+      <c r="F130" t="s">
+        <v>238</v>
+      </c>
+      <c r="G130" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>144</v>
+      </c>
+      <c r="B131" t="s">
+        <v>239</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>327</v>
+      </c>
+      <c r="F131" t="s">
+        <v>240</v>
+      </c>
+      <c r="G131" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>145</v>
+      </c>
+      <c r="B132" t="s">
+        <v>241</v>
+      </c>
+      <c r="C132" t="s">
+        <v>32</v>
+      </c>
+      <c r="E132">
+        <v>328</v>
+      </c>
+      <c r="F132" t="s">
+        <v>242</v>
+      </c>
+      <c r="G132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>146</v>
+      </c>
+      <c r="B133" t="s">
+        <v>243</v>
+      </c>
+      <c r="C133" t="s">
+        <v>32</v>
+      </c>
+      <c r="E133">
+        <v>329</v>
+      </c>
+      <c r="F133" t="s">
+        <v>244</v>
+      </c>
+      <c r="G133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>147</v>
+      </c>
+      <c r="B134" t="s">
+        <v>245</v>
+      </c>
+      <c r="C134" t="s">
+        <v>32</v>
+      </c>
+      <c r="E134">
+        <v>330</v>
+      </c>
+      <c r="F134" t="s">
+        <v>246</v>
+      </c>
+      <c r="G134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>148</v>
+      </c>
+      <c r="B135" t="s">
+        <v>247</v>
+      </c>
+      <c r="C135" t="s">
+        <v>32</v>
+      </c>
+      <c r="E135">
+        <v>331</v>
+      </c>
+      <c r="F135" t="s">
+        <v>248</v>
+      </c>
+      <c r="G135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>150</v>
+      </c>
+      <c r="B136" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="C136" s="5">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>333</v>
+      </c>
+      <c r="F136" t="s">
+        <v>346</v>
+      </c>
+      <c r="G136" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>151</v>
+      </c>
+      <c r="B137" t="s">
+        <v>347</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="E137">
+        <v>334</v>
+      </c>
+      <c r="F137" t="s">
+        <v>348</v>
+      </c>
+      <c r="G137" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>152</v>
+      </c>
+      <c r="B138" t="s">
+        <v>349</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="E138">
+        <v>335</v>
+      </c>
+      <c r="F138" t="s">
+        <v>350</v>
+      </c>
+      <c r="G138" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>153</v>
+      </c>
+      <c r="B139" t="s">
+        <v>351</v>
+      </c>
+      <c r="C139" t="s">
+        <v>32</v>
+      </c>
+      <c r="E139">
+        <v>336</v>
+      </c>
+      <c r="F139" t="s">
+        <v>352</v>
+      </c>
+      <c r="G139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>154</v>
+      </c>
+      <c r="B140" t="s">
+        <v>353</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="E140">
+        <v>337</v>
+      </c>
+      <c r="F140" t="s">
+        <v>354</v>
+      </c>
+      <c r="G140" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>155</v>
+      </c>
+      <c r="B141" t="s">
+        <v>355</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="E141">
+        <v>338</v>
+      </c>
+      <c r="F141" t="s">
+        <v>356</v>
+      </c>
+      <c r="G141" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>156</v>
+      </c>
+      <c r="B142" t="s">
+        <v>357</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>339</v>
+      </c>
+      <c r="F142" t="s">
+        <v>358</v>
+      </c>
+      <c r="G142" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>157</v>
+      </c>
+      <c r="B143" t="s">
+        <v>359</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="E143">
+        <v>340</v>
+      </c>
+      <c r="F143" t="s">
+        <v>360</v>
+      </c>
+      <c r="G143" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>159</v>
+      </c>
+      <c r="B144" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C144" s="5">
+        <v>1</v>
+      </c>
+      <c r="E144">
+        <v>342</v>
+      </c>
+      <c r="F144" t="s">
+        <v>266</v>
+      </c>
+      <c r="G144" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>160</v>
+      </c>
+      <c r="B145" t="s">
+        <v>267</v>
+      </c>
+      <c r="C145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>343</v>
+      </c>
+      <c r="F145" t="s">
+        <v>268</v>
+      </c>
+      <c r="G145" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <v>161</v>
+      </c>
+      <c r="B146" t="s">
+        <v>269</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="E146">
+        <v>344</v>
+      </c>
+      <c r="F146" t="s">
+        <v>270</v>
+      </c>
+      <c r="G146" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <v>162</v>
+      </c>
+      <c r="B147" t="s">
+        <v>271</v>
+      </c>
+      <c r="C147" t="s">
+        <v>32</v>
+      </c>
+      <c r="E147">
+        <v>345</v>
+      </c>
+      <c r="F147" t="s">
+        <v>272</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <v>163</v>
+      </c>
+      <c r="B148" t="s">
+        <v>273</v>
+      </c>
+      <c r="C148" t="s">
+        <v>32</v>
+      </c>
+      <c r="E148">
+        <v>346</v>
+      </c>
+      <c r="F148" t="s">
+        <v>274</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <v>164</v>
+      </c>
+      <c r="B149" t="s">
+        <v>275</v>
+      </c>
+      <c r="C149">
+        <v>1</v>
+      </c>
+      <c r="E149">
+        <v>347</v>
+      </c>
+      <c r="F149" t="s">
+        <v>276</v>
+      </c>
+      <c r="G149" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <v>165</v>
+      </c>
+      <c r="B150" t="s">
+        <v>277</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="E150">
+        <v>348</v>
+      </c>
+      <c r="F150" t="s">
+        <v>278</v>
+      </c>
+      <c r="G150" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>166</v>
+      </c>
+      <c r="B151" t="s">
+        <v>279</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>349</v>
+      </c>
+      <c r="F151" t="s">
+        <v>280</v>
+      </c>
+      <c r="G151" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>168</v>
+      </c>
+      <c r="B152" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="C152" s="5">
+        <v>1</v>
+      </c>
+      <c r="E152">
+        <v>351</v>
+      </c>
+      <c r="F152" t="s">
+        <v>281</v>
+      </c>
+      <c r="G152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>169</v>
+      </c>
+      <c r="B153" t="s">
+        <v>284</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
+      <c r="E153">
+        <v>352</v>
+      </c>
+      <c r="F153" t="s">
+        <v>283</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>170</v>
+      </c>
+      <c r="B154" t="s">
+        <v>286</v>
+      </c>
+      <c r="C154" t="s">
+        <v>32</v>
+      </c>
+      <c r="E154">
+        <v>353</v>
+      </c>
+      <c r="F154" t="s">
+        <v>285</v>
+      </c>
+      <c r="G154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>171</v>
+      </c>
+      <c r="B155" t="s">
+        <v>288</v>
+      </c>
+      <c r="C155" t="s">
+        <v>32</v>
+      </c>
+      <c r="E155">
+        <v>354</v>
+      </c>
+      <c r="F155" t="s">
+        <v>287</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>172</v>
+      </c>
+      <c r="B156" t="s">
+        <v>290</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+      <c r="E156">
+        <v>355</v>
+      </c>
+      <c r="F156" t="s">
+        <v>289</v>
+      </c>
+      <c r="G156" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>173</v>
+      </c>
+      <c r="B157" t="s">
+        <v>292</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="E157">
+        <v>356</v>
+      </c>
+      <c r="F157" t="s">
+        <v>291</v>
+      </c>
+      <c r="G157" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>174</v>
+      </c>
+      <c r="B158" t="s">
+        <v>294</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="E158">
+        <v>357</v>
+      </c>
+      <c r="F158" t="s">
+        <v>293</v>
+      </c>
+      <c r="G158" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>175</v>
+      </c>
+      <c r="B159" t="s">
+        <v>296</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="E159">
+        <v>358</v>
+      </c>
+      <c r="F159" t="s">
+        <v>295</v>
+      </c>
+      <c r="G159" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>177</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="C160" s="5">
+        <v>1</v>
+      </c>
+      <c r="E160">
+        <v>360</v>
+      </c>
+      <c r="F160" t="s">
+        <v>298</v>
+      </c>
+      <c r="G160" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>178</v>
+      </c>
+      <c r="B161" t="s">
+        <v>299</v>
+      </c>
+      <c r="C161">
+        <v>1</v>
+      </c>
+      <c r="E161">
+        <v>361</v>
+      </c>
+      <c r="F161" t="s">
+        <v>300</v>
+      </c>
+      <c r="G161" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>179</v>
+      </c>
+      <c r="B162" t="s">
+        <v>301</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+      <c r="E162">
+        <v>362</v>
+      </c>
+      <c r="F162" t="s">
+        <v>302</v>
+      </c>
+      <c r="G162" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A163">
+        <v>180</v>
+      </c>
+      <c r="B163" t="s">
+        <v>303</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+      <c r="E163">
+        <v>363</v>
+      </c>
+      <c r="F163" t="s">
+        <v>304</v>
+      </c>
+      <c r="G163" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A164">
+        <v>181</v>
+      </c>
+      <c r="B164" t="s">
+        <v>305</v>
+      </c>
+      <c r="C164" t="s">
+        <v>32</v>
+      </c>
+      <c r="E164">
+        <v>364</v>
+      </c>
+      <c r="F164" t="s">
+        <v>306</v>
+      </c>
+      <c r="G164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A165">
+        <v>182</v>
+      </c>
+      <c r="B165" t="s">
+        <v>307</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+      <c r="E165">
+        <v>365</v>
+      </c>
+      <c r="F165" t="s">
+        <v>308</v>
+      </c>
+      <c r="G165" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>183</v>
+      </c>
+      <c r="B166" t="s">
+        <v>309</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+      <c r="E166">
+        <v>366</v>
+      </c>
+      <c r="F166" t="s">
+        <v>310</v>
+      </c>
+      <c r="G166" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>184</v>
+      </c>
+      <c r="B167" t="s">
+        <v>311</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+      <c r="E167">
+        <v>367</v>
+      </c>
+      <c r="F167" t="s">
+        <v>312</v>
+      </c>
+      <c r="G167" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>186</v>
+      </c>
+      <c r="B168" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C168" s="5">
+        <v>1</v>
+      </c>
+      <c r="E168">
+        <v>369</v>
+      </c>
+      <c r="F168" t="s">
+        <v>313</v>
+      </c>
+      <c r="G168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>187</v>
+      </c>
+      <c r="B169" t="s">
+        <v>316</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="E169">
+        <v>370</v>
+      </c>
+      <c r="F169" t="s">
+        <v>315</v>
+      </c>
+      <c r="G169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>188</v>
+      </c>
+      <c r="B170" t="s">
+        <v>318</v>
+      </c>
+      <c r="C170" t="s">
+        <v>32</v>
+      </c>
+      <c r="E170">
+        <v>371</v>
+      </c>
+      <c r="F170" t="s">
+        <v>317</v>
+      </c>
+      <c r="G170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>189</v>
+      </c>
+      <c r="B171" t="s">
+        <v>320</v>
+      </c>
+      <c r="C171" t="s">
+        <v>32</v>
+      </c>
+      <c r="E171">
+        <v>372</v>
+      </c>
+      <c r="F171" t="s">
+        <v>319</v>
+      </c>
+      <c r="G171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>190</v>
+      </c>
+      <c r="B172" t="s">
+        <v>322</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="E172">
+        <v>373</v>
+      </c>
+      <c r="F172" t="s">
+        <v>321</v>
+      </c>
+      <c r="G172" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A173">
+        <v>191</v>
+      </c>
+      <c r="B173" t="s">
+        <v>324</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+      <c r="E173">
+        <v>374</v>
+      </c>
+      <c r="F173" t="s">
+        <v>323</v>
+      </c>
+      <c r="G173" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A174">
+        <v>192</v>
+      </c>
+      <c r="B174" t="s">
+        <v>326</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>375</v>
+      </c>
+      <c r="F174" t="s">
+        <v>325</v>
+      </c>
+      <c r="G174" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A175">
+        <v>193</v>
+      </c>
+      <c r="B175" t="s">
+        <v>328</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>376</v>
+      </c>
+      <c r="F175" t="s">
+        <v>327</v>
+      </c>
+      <c r="G175" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A176">
+        <v>195</v>
+      </c>
+      <c r="B176" t="s">
+        <v>329</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>378</v>
+      </c>
+      <c r="F176" t="s">
+        <v>330</v>
+      </c>
+      <c r="G176" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>196</v>
+      </c>
+      <c r="B177" t="s">
+        <v>331</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>379</v>
+      </c>
+      <c r="F177" t="s">
+        <v>332</v>
+      </c>
+      <c r="G177" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>197</v>
+      </c>
+      <c r="B178" t="s">
+        <v>333</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+      <c r="E178">
+        <v>380</v>
+      </c>
+      <c r="F178" t="s">
+        <v>334</v>
+      </c>
+      <c r="G178" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>198</v>
+      </c>
+      <c r="B179" t="s">
+        <v>335</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>381</v>
+      </c>
+      <c r="F179" t="s">
+        <v>336</v>
+      </c>
+      <c r="G179" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>199</v>
+      </c>
+      <c r="B180" t="s">
+        <v>337</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>382</v>
+      </c>
+      <c r="F180" t="s">
+        <v>338</v>
+      </c>
+      <c r="G180" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>200</v>
+      </c>
+      <c r="B181" t="s">
+        <v>339</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="E181">
+        <v>383</v>
+      </c>
+      <c r="F181" t="s">
+        <v>340</v>
+      </c>
+      <c r="G181" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>201</v>
+      </c>
+      <c r="B182" t="s">
+        <v>341</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="E182">
+        <v>384</v>
+      </c>
+      <c r="F182" t="s">
+        <v>342</v>
+      </c>
+      <c r="G182" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>202</v>
+      </c>
+      <c r="B183" t="s">
+        <v>343</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="E183">
+        <v>385</v>
+      </c>
+      <c r="F183" t="s">
+        <v>344</v>
+      </c>
+      <c r="G183" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>204</v>
+      </c>
+      <c r="B184" t="s">
+        <v>381</v>
+      </c>
+      <c r="C184" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>205</v>
+      </c>
+      <c r="B185" t="s">
+        <v>380</v>
+      </c>
+      <c r="C185" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>206</v>
+      </c>
+      <c r="B186" t="s">
+        <v>379</v>
+      </c>
+      <c r="C186" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>207</v>
+      </c>
+      <c r="B187" t="s">
+        <v>378</v>
+      </c>
+      <c r="C187" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>208</v>
+      </c>
+      <c r="B188" t="s">
+        <v>377</v>
+      </c>
+      <c r="C188" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>209</v>
+      </c>
+      <c r="B189" t="s">
+        <v>376</v>
+      </c>
+      <c r="C189" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>210</v>
+      </c>
+      <c r="B190" t="s">
+        <v>375</v>
+      </c>
+      <c r="C190" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>211</v>
+      </c>
+      <c r="B191" t="s">
+        <v>374</v>
+      </c>
+      <c r="C191" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G191" xr:uid="{5858AF94-AA92-4F75-9184-ED8ECFD866A0}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>